<commit_message>
chore: update Excel files and test data
- Update Excel files in src/data/storage
- Add new test data images and Excel files
- Update compiled Python files in __pycache__
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_img_input.xlsx
+++ b/src/data/input/manual/temp_img_input.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="13368" yWindow="3444" windowWidth="18264" windowHeight="12156" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -18,18 +18,17 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -41,27 +40,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -70,12 +54,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -441,11 +423,15 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" activeCellId="1" sqref="A3:J5 B2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="11.6640625" bestFit="1" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(app): - finished:   - 完成打包工作 - todo:   - 解决打包运行的报错
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_img_input.xlsx
+++ b/src/data/input/manual/temp_img_input.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -18,18 +19,14 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <family val="3"/>
-      <sz val="9"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,15 +45,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -421,15 +427,11 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
-  <cols>
-    <col width="17.81640625" customWidth="1" min="4" max="4"/>
-    <col width="17.81640625" customWidth="1" min="13" max="13"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Unicode documentation, update file paths, and add DLL handling script
- Created a new documentation file for Unicode escape sequences in Python, explaining the usage of `\u` and `\U` for Unicode characters.
- Added a new Python script to handle the addition of DLL directories for Paddle.
- Updated file paths in the main window GUI code to use relative paths instead of absolute paths for better portability.
- Added several binary files and Excel files to the storage backup directory.
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_img_input.xlsx
+++ b/src/data/input/manual/temp_img_input.xlsx
@@ -425,14 +425,571 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>日期</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>类别</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>品名</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>单位</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>数量</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>单价</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>金额</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>备注</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>公司</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>单名</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>油麦菜1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>桶</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>24.87</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>49.74</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>老抽2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>桶</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>18.15</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>36.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>辣椒粉10</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2.88</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>57.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>桶</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>22.02</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>44.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>捞汁2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>郫县豆瓣酱7</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>4.22</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>21.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>十三香10</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>盒</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>3.33</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>66.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>粉丝10</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>5.72</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>57.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>芝麻6</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1.89</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>18.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>孜然10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2 73</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>27.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2.88</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>57.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>挂面25</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>辣椒粉10</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2.88</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>28.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>粉丝10</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>10.94</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>54.7</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>香琪酱20</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>1.64</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>32.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>扶贫木耳</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>斤</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>61.69</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>123.38</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>麻辣鲜</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2.63</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>26.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>25.86</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>火锅底料</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>12.93</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>方便面 (104g)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>袋</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2.38</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>23.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>料酒14</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>车 机招餐</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>4.97</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>49.7</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>糖三角</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>宏程餐饮</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>管</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>